<commit_message>
text size and position in labels update
</commit_message>
<xml_diff>
--- a/Metadata2.xlsx
+++ b/Metadata2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngiordano\OneDrive - Kansas State University\Desktop\KSU-WHEAT-APP-main-2.0\IDataField-2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A4F9DD-4BB7-4037-B26F-F290F61E5F23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E508F703-8977-4765-ADBB-315E1B9C7905}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23148" windowHeight="9888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23148" windowHeight="9888" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experimental Designs" sheetId="9" r:id="rId1"/>
@@ -697,9 +697,6 @@
     <t>PS, F3</t>
   </si>
   <si>
-    <t>ACTIVITY_SHORT name</t>
-  </si>
-  <si>
     <t>NFU</t>
   </si>
   <si>
@@ -755,6 +752,9 @@
   </si>
   <si>
     <t>TC</t>
+  </si>
+  <si>
+    <t>ACTIVITY_SHORT</t>
   </si>
 </sst>
 </file>
@@ -1647,8 +1647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E757A881-E26C-4178-B684-57531D1649A8}">
   <dimension ref="A1:G285"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView topLeftCell="A255" workbookViewId="0">
+      <selection activeCell="I271" sqref="I271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -8217,8 +8217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -8825,8 +8825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA34306-CC0E-404E-B174-25F87B7E0796}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -9132,8 +9132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CF72BDF-E972-4DFC-8739-BD42FEEE886B}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -9147,7 +9147,7 @@
         <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -9155,7 +9155,7 @@
         <v>206</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -9163,7 +9163,7 @@
         <v>207</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -9179,7 +9179,7 @@
         <v>210</v>
       </c>
       <c r="B5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -9215,82 +9215,82 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -9333,7 +9333,7 @@
         <v>216</v>
       </c>
       <c r="B3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -9342,23 +9342,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="360d84ef-15ff-4e17-9c6b-a1028cb8e8ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004985193A87153942845D241572937CE5" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="41d807227133e919f3755c54a0ed2601">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="360d84ef-15ff-4e17-9c6b-a1028cb8e8ff" xmlns:ns4="f703b2de-b014-43d1-91b4-4178b52ec481" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="28768a436f2ded89381638814bc7efce" ns3:_="" ns4:_="">
     <xsd:import namespace="360d84ef-15ff-4e17-9c6b-a1028cb8e8ff"/>
@@ -9599,25 +9582,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80E2AB2F-6E1F-424C-8E97-B29CFF39A56D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="360d84ef-15ff-4e17-9c6b-a1028cb8e8ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{309818C2-C029-41E7-90B5-C5C7A9CD1F23}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="360d84ef-15ff-4e17-9c6b-a1028cb8e8ff"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3154782E-A8FB-4B5D-908B-67EB26D31F14}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9634,4 +9616,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{309818C2-C029-41E7-90B5-C5C7A9CD1F23}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="360d84ef-15ff-4e17-9c6b-a1028cb8e8ff"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80E2AB2F-6E1F-424C-8E97-B29CFF39A56D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>